<commit_message>
Update files and calendar (2026-01-26 18:53:40 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2026.xlsx
+++ b/files/IT_2026.xlsx
@@ -11,7 +11,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{991245FC-07BC-4015-BDEF-4EED57848F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="11" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN" sheetId="86" r:id="rId1"/>
@@ -802,6 +802,33 @@
     <xf numFmtId="0" fontId="4" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -817,31 +844,10 @@
     <xf numFmtId="17" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -855,12 +861,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1592,8 +1592,8 @@
   <dimension ref="A1:AN30"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="W4" sqref="W4"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AE5" sqref="AE5"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -1606,40 +1606,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="56"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
@@ -1650,7 +1650,7 @@
       <c r="AN1" s="12"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="48">
+      <c r="A2" s="57">
         <v>46023</v>
       </c>
       <c r="B2" s="23">
@@ -1777,19 +1777,19 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="50"/>
-      <c r="AJ2" s="50"/>
-      <c r="AL2" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="50"/>
-      <c r="AN2" s="50"/>
+      <c r="AH2" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="45"/>
+      <c r="AL2" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="45"/>
+      <c r="AN2" s="45"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1">
-      <c r="A3" s="48"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="23" t="str">
         <f t="shared" ref="B3:AF3" si="1">UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>TH</v>
@@ -2144,8 +2144,8 @@
       <c r="AD5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AE5" s="3" t="s">
-        <v>11</v>
+      <c r="AE5" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="AF5" s="14" t="s">
         <v>8</v>
@@ -2866,8 +2866,8 @@
       <c r="AD11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AE11" s="14" t="s">
-        <v>8</v>
+      <c r="AE11" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="AF11" s="14" t="s">
         <v>8</v>
@@ -3156,14 +3156,14 @@
     <row r="15" spans="1:40" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:40">
       <c r="E16" s="42"/>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="55" t="s">
+      <c r="G16" s="59"/>
+      <c r="H16" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="62"/>
+      <c r="I16" s="47"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -3184,28 +3184,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="58" t="s">
+      <c r="Z16" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="59"/>
-      <c r="AD16" s="59"/>
-      <c r="AE16" s="59"/>
-      <c r="AF16" s="59"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="61"/>
+      <c r="AE16" s="61"/>
+      <c r="AF16" s="61"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51" t="s">
+      <c r="G17" s="58"/>
+      <c r="H17" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="63"/>
+      <c r="I17" s="49"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -3226,26 +3226,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="61"/>
-      <c r="AD17" s="61"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="61"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="63"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="63"/>
+      <c r="AE17" s="63"/>
+      <c r="AF17" s="63"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="53" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="57"/>
+      <c r="I18" s="51"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -3266,26 +3266,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="61"/>
-      <c r="AD18" s="61"/>
-      <c r="AE18" s="61"/>
-      <c r="AF18" s="61"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="63"/>
+      <c r="AC18" s="63"/>
+      <c r="AD18" s="63"/>
+      <c r="AE18" s="63"/>
+      <c r="AF18" s="63"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="54"/>
-      <c r="H19" s="53" t="s">
+      <c r="G19" s="52"/>
+      <c r="H19" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="57"/>
+      <c r="I19" s="51"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -3311,14 +3311,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="57"/>
+      <c r="I20" s="51"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -3344,14 +3344,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="44" t="s">
+      <c r="G21" s="54"/>
+      <c r="H21" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="46"/>
+      <c r="I21" s="55"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -3573,12 +3573,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="A1:AF1"/>
@@ -3590,6 +3584,12 @@
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="Z16:AF18"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
   </mergeCells>
   <conditionalFormatting sqref="B13:AF14">
     <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
@@ -3628,47 +3628,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="56"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="48">
+      <c r="A2" s="57">
         <v>46296</v>
       </c>
       <c r="B2" s="21">
@@ -3795,14 +3795,14 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="50"/>
-      <c r="AJ2" s="50"/>
+      <c r="AH2" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="45"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="48"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>TH</v>
@@ -5079,14 +5079,14 @@
     <row r="15" spans="1:36" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:36">
       <c r="E16" s="42"/>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="55" t="s">
+      <c r="G16" s="59"/>
+      <c r="H16" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="62"/>
+      <c r="I16" s="47"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -5107,28 +5107,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="58" t="s">
+      <c r="Z16" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="59"/>
-      <c r="AD16" s="59"/>
-      <c r="AE16" s="59"/>
-      <c r="AF16" s="59"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="61"/>
+      <c r="AE16" s="61"/>
+      <c r="AF16" s="61"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51" t="s">
+      <c r="G17" s="58"/>
+      <c r="H17" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="63"/>
+      <c r="I17" s="49"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -5149,26 +5149,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="61"/>
-      <c r="AD17" s="61"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="61"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="63"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="63"/>
+      <c r="AE17" s="63"/>
+      <c r="AF17" s="63"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="53" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="57"/>
+      <c r="I18" s="51"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -5189,26 +5189,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="61"/>
-      <c r="AD18" s="61"/>
-      <c r="AE18" s="61"/>
-      <c r="AF18" s="61"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="63"/>
+      <c r="AC18" s="63"/>
+      <c r="AD18" s="63"/>
+      <c r="AE18" s="63"/>
+      <c r="AF18" s="63"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="54"/>
-      <c r="H19" s="53" t="s">
+      <c r="G19" s="52"/>
+      <c r="H19" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="57"/>
+      <c r="I19" s="51"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -5234,14 +5234,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="57"/>
+      <c r="I20" s="51"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -5267,14 +5267,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="44" t="s">
+      <c r="G21" s="54"/>
+      <c r="H21" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="46"/>
+      <c r="I21" s="55"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -5496,12 +5496,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -5512,6 +5506,12 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:E3 G2:AF3">
     <cfRule type="expression" dxfId="8" priority="3">
@@ -5550,46 +5550,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
       <c r="AF1" s="12"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="48">
+      <c r="A2" s="57">
         <v>46327</v>
       </c>
       <c r="B2" s="23">
@@ -5712,14 +5712,14 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AG2" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="50"/>
-      <c r="AI2" s="50"/>
+      <c r="AG2" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="45"/>
+      <c r="AI2" s="45"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1">
-      <c r="A3" s="48"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="23" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>SU</v>
@@ -6960,14 +6960,14 @@
     <row r="15" spans="1:35" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:35">
       <c r="E16" s="42"/>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="55" t="s">
+      <c r="G16" s="59"/>
+      <c r="H16" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="62"/>
+      <c r="I16" s="47"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -6988,28 +6988,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="58" t="s">
+      <c r="Z16" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="59"/>
-      <c r="AD16" s="59"/>
-      <c r="AE16" s="59"/>
-      <c r="AF16" s="59"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="61"/>
+      <c r="AE16" s="61"/>
+      <c r="AF16" s="61"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51" t="s">
+      <c r="G17" s="58"/>
+      <c r="H17" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="63"/>
+      <c r="I17" s="49"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -7030,26 +7030,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="61"/>
-      <c r="AD17" s="61"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="61"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="63"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="63"/>
+      <c r="AE17" s="63"/>
+      <c r="AF17" s="63"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="53" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="57"/>
+      <c r="I18" s="51"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -7070,26 +7070,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="61"/>
-      <c r="AD18" s="61"/>
-      <c r="AE18" s="61"/>
-      <c r="AF18" s="61"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="63"/>
+      <c r="AC18" s="63"/>
+      <c r="AD18" s="63"/>
+      <c r="AE18" s="63"/>
+      <c r="AF18" s="63"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="54"/>
-      <c r="H19" s="53" t="s">
+      <c r="G19" s="52"/>
+      <c r="H19" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="57"/>
+      <c r="I19" s="51"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -7115,14 +7115,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="57"/>
+      <c r="I20" s="51"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -7148,14 +7148,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="44" t="s">
+      <c r="G21" s="54"/>
+      <c r="H21" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="46"/>
+      <c r="I21" s="55"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -7377,12 +7377,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -7393,6 +7387,12 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B13:AE14">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
@@ -7416,7 +7416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4661035D-4F15-4FC2-8B47-A29E37BFBC5D}">
   <dimension ref="A1:AJ30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="AI19" sqref="AI19"/>
       <selection pane="bottomLeft"/>
@@ -7431,47 +7431,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="56"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="48">
+      <c r="A2" s="57">
         <v>46357</v>
       </c>
       <c r="B2" s="23">
@@ -7598,14 +7598,14 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="50"/>
-      <c r="AJ2" s="50"/>
+      <c r="AH2" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="45"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="48"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="23" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>TU</v>
@@ -8882,14 +8882,14 @@
     <row r="15" spans="1:36" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:36">
       <c r="E16" s="42"/>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="55" t="s">
+      <c r="G16" s="59"/>
+      <c r="H16" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="62"/>
+      <c r="I16" s="47"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -8910,28 +8910,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="58" t="s">
+      <c r="Z16" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="59"/>
-      <c r="AD16" s="59"/>
-      <c r="AE16" s="59"/>
-      <c r="AF16" s="59"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="61"/>
+      <c r="AE16" s="61"/>
+      <c r="AF16" s="61"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51" t="s">
+      <c r="G17" s="58"/>
+      <c r="H17" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="63"/>
+      <c r="I17" s="49"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -8952,26 +8952,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="61"/>
-      <c r="AD17" s="61"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="61"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="63"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="63"/>
+      <c r="AE17" s="63"/>
+      <c r="AF17" s="63"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="53" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="57"/>
+      <c r="I18" s="51"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -8992,26 +8992,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="61"/>
-      <c r="AD18" s="61"/>
-      <c r="AE18" s="61"/>
-      <c r="AF18" s="61"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="63"/>
+      <c r="AC18" s="63"/>
+      <c r="AD18" s="63"/>
+      <c r="AE18" s="63"/>
+      <c r="AF18" s="63"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="54"/>
-      <c r="H19" s="53" t="s">
+      <c r="G19" s="52"/>
+      <c r="H19" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="57"/>
+      <c r="I19" s="51"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -9037,14 +9037,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="57"/>
+      <c r="I20" s="51"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -9070,14 +9070,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="44" t="s">
+      <c r="G21" s="54"/>
+      <c r="H21" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="46"/>
+      <c r="I21" s="55"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -9299,12 +9299,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -9315,6 +9309,12 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B13:AF14">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -9338,9 +9338,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E901B9E-1F8C-4966-83E5-6829517B3DD1}">
   <dimension ref="A1:AK30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -9353,37 +9353,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
       <c r="AD1" s="12"/>
       <c r="AE1" s="12"/>
       <c r="AF1" s="12"/>
@@ -9394,7 +9394,7 @@
       <c r="AK1" s="12"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="48">
+      <c r="A2" s="57">
         <v>46054</v>
       </c>
       <c r="B2" s="21">
@@ -9509,19 +9509,19 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AE2" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="50"/>
-      <c r="AG2" s="50"/>
-      <c r="AI2" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="50"/>
-      <c r="AK2" s="50"/>
+      <c r="AE2" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="45"/>
+      <c r="AG2" s="45"/>
+      <c r="AI2" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="45"/>
+      <c r="AK2" s="45"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1">
-      <c r="A3" s="48"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>SU</v>
@@ -10450,8 +10450,8 @@
       <c r="A11" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>16</v>
+      <c r="B11" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>16</v>
@@ -10682,7 +10682,7 @@
       </c>
       <c r="B14" s="14">
         <f>COUNTIF(B4:B11,"P14")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="14">
         <f t="shared" ref="C14:AC14" si="7">COUNTIF(C4:C11,"P14")</f>
@@ -10796,14 +10796,14 @@
     <row r="15" spans="1:37" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:37">
       <c r="E16" s="42"/>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="55" t="s">
+      <c r="G16" s="59"/>
+      <c r="H16" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="62"/>
+      <c r="I16" s="47"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -10824,28 +10824,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="58" t="s">
+      <c r="Z16" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="59"/>
-      <c r="AD16" s="59"/>
-      <c r="AE16" s="59"/>
-      <c r="AF16" s="59"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="61"/>
+      <c r="AE16" s="61"/>
+      <c r="AF16" s="61"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51" t="s">
+      <c r="G17" s="58"/>
+      <c r="H17" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="63"/>
+      <c r="I17" s="49"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -10866,26 +10866,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="61"/>
-      <c r="AD17" s="61"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="61"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="63"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="63"/>
+      <c r="AE17" s="63"/>
+      <c r="AF17" s="63"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="53" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="57"/>
+      <c r="I18" s="51"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -10906,26 +10906,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="61"/>
-      <c r="AD18" s="61"/>
-      <c r="AE18" s="61"/>
-      <c r="AF18" s="61"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="63"/>
+      <c r="AC18" s="63"/>
+      <c r="AD18" s="63"/>
+      <c r="AE18" s="63"/>
+      <c r="AF18" s="63"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="54"/>
-      <c r="H19" s="53" t="s">
+      <c r="G19" s="52"/>
+      <c r="H19" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="57"/>
+      <c r="I19" s="51"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -10951,14 +10951,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="57"/>
+      <c r="I20" s="51"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -10984,14 +10984,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="44" t="s">
+      <c r="G21" s="54"/>
+      <c r="H21" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="46"/>
+      <c r="I21" s="55"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -11213,13 +11213,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:AC1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -11230,6 +11223,13 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A1:AC1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:Q3 S2:AC3">
     <cfRule type="expression" dxfId="32" priority="5">
@@ -11268,40 +11268,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="56"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
@@ -11312,7 +11312,7 @@
       <c r="AN1" s="12"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="48">
+      <c r="A2" s="57">
         <v>46082</v>
       </c>
       <c r="B2" s="21">
@@ -11439,19 +11439,19 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="50"/>
-      <c r="AJ2" s="50"/>
-      <c r="AL2" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="50"/>
-      <c r="AN2" s="50"/>
+      <c r="AH2" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="45"/>
+      <c r="AL2" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="45"/>
+      <c r="AN2" s="45"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1">
-      <c r="A3" s="48"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>SU</v>
@@ -12834,14 +12834,14 @@
     <row r="15" spans="1:40" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:40">
       <c r="E16" s="42"/>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="55" t="s">
+      <c r="G16" s="59"/>
+      <c r="H16" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="62"/>
+      <c r="I16" s="47"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -12862,28 +12862,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="58" t="s">
+      <c r="Z16" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="59"/>
-      <c r="AD16" s="59"/>
-      <c r="AE16" s="59"/>
-      <c r="AF16" s="59"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="61"/>
+      <c r="AE16" s="61"/>
+      <c r="AF16" s="61"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51" t="s">
+      <c r="G17" s="58"/>
+      <c r="H17" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="63"/>
+      <c r="I17" s="49"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -12904,26 +12904,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="61"/>
-      <c r="AD17" s="61"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="61"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="63"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="63"/>
+      <c r="AE17" s="63"/>
+      <c r="AF17" s="63"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="53" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="57"/>
+      <c r="I18" s="51"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -12944,26 +12944,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="61"/>
-      <c r="AD18" s="61"/>
-      <c r="AE18" s="61"/>
-      <c r="AF18" s="61"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="63"/>
+      <c r="AC18" s="63"/>
+      <c r="AD18" s="63"/>
+      <c r="AE18" s="63"/>
+      <c r="AF18" s="63"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="54"/>
-      <c r="H19" s="53" t="s">
+      <c r="G19" s="52"/>
+      <c r="H19" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="57"/>
+      <c r="I19" s="51"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -12989,14 +12989,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="57"/>
+      <c r="I20" s="51"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -13022,14 +13022,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="44" t="s">
+      <c r="G21" s="54"/>
+      <c r="H21" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="46"/>
+      <c r="I21" s="55"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -13251,13 +13251,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -13268,6 +13261,13 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:AF3">
     <cfRule type="expression" dxfId="29" priority="5">
@@ -13306,39 +13306,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
       <c r="AF1" s="12"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
@@ -13349,7 +13349,7 @@
       <c r="AM1" s="12"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
-      <c r="A2" s="48">
+      <c r="A2" s="57">
         <v>46113</v>
       </c>
       <c r="B2" s="21">
@@ -13472,19 +13472,19 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AG2" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="50"/>
-      <c r="AI2" s="50"/>
-      <c r="AK2" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="50"/>
-      <c r="AM2" s="50"/>
+      <c r="AG2" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="45"/>
+      <c r="AI2" s="45"/>
+      <c r="AK2" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="45"/>
+      <c r="AM2" s="45"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1">
-      <c r="A3" s="48"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>WE</v>
@@ -14831,14 +14831,14 @@
     <row r="15" spans="1:39" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:39">
       <c r="E16" s="42"/>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="55" t="s">
+      <c r="G16" s="59"/>
+      <c r="H16" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="62"/>
+      <c r="I16" s="47"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -14859,28 +14859,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="58" t="s">
+      <c r="Z16" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="59"/>
-      <c r="AD16" s="59"/>
-      <c r="AE16" s="59"/>
-      <c r="AF16" s="59"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="61"/>
+      <c r="AE16" s="61"/>
+      <c r="AF16" s="61"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51" t="s">
+      <c r="G17" s="58"/>
+      <c r="H17" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="63"/>
+      <c r="I17" s="49"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -14901,26 +14901,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="61"/>
-      <c r="AD17" s="61"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="61"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="63"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="63"/>
+      <c r="AE17" s="63"/>
+      <c r="AF17" s="63"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="53" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="57"/>
+      <c r="I18" s="51"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -14941,26 +14941,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="61"/>
-      <c r="AD18" s="61"/>
-      <c r="AE18" s="61"/>
-      <c r="AF18" s="61"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="63"/>
+      <c r="AC18" s="63"/>
+      <c r="AD18" s="63"/>
+      <c r="AE18" s="63"/>
+      <c r="AF18" s="63"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="54"/>
-      <c r="H19" s="53" t="s">
+      <c r="G19" s="52"/>
+      <c r="H19" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="57"/>
+      <c r="I19" s="51"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -14986,14 +14986,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="57"/>
+      <c r="I20" s="51"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -15019,14 +15019,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="44" t="s">
+      <c r="G21" s="54"/>
+      <c r="H21" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="46"/>
+      <c r="I21" s="55"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -15248,13 +15248,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -15265,6 +15258,13 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="AK2:AM2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:C3 E2:E3 G2:Y3 AA2:AE3">
     <cfRule type="expression" dxfId="26" priority="3">
@@ -15303,47 +15303,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="56"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="48">
+      <c r="A2" s="57">
         <v>46143</v>
       </c>
       <c r="B2" s="23">
@@ -15470,14 +15470,14 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="50"/>
-      <c r="AJ2" s="50"/>
+      <c r="AH2" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="45"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="48"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="23" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>FR</v>
@@ -16754,14 +16754,14 @@
     <row r="15" spans="1:36" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:36">
       <c r="E16" s="42"/>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="55" t="s">
+      <c r="G16" s="59"/>
+      <c r="H16" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="62"/>
+      <c r="I16" s="47"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -16782,28 +16782,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="58" t="s">
+      <c r="Z16" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="59"/>
-      <c r="AD16" s="59"/>
-      <c r="AE16" s="59"/>
-      <c r="AF16" s="59"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="61"/>
+      <c r="AE16" s="61"/>
+      <c r="AF16" s="61"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51" t="s">
+      <c r="G17" s="58"/>
+      <c r="H17" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="63"/>
+      <c r="I17" s="49"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -16824,26 +16824,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="61"/>
-      <c r="AD17" s="61"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="61"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="63"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="63"/>
+      <c r="AE17" s="63"/>
+      <c r="AF17" s="63"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="53" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="57"/>
+      <c r="I18" s="51"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -16864,26 +16864,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="61"/>
-      <c r="AD18" s="61"/>
-      <c r="AE18" s="61"/>
-      <c r="AF18" s="61"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="63"/>
+      <c r="AC18" s="63"/>
+      <c r="AD18" s="63"/>
+      <c r="AE18" s="63"/>
+      <c r="AF18" s="63"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="54"/>
-      <c r="H19" s="53" t="s">
+      <c r="G19" s="52"/>
+      <c r="H19" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="57"/>
+      <c r="I19" s="51"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -16909,14 +16909,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="57"/>
+      <c r="I20" s="51"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -16942,14 +16942,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="44" t="s">
+      <c r="G21" s="54"/>
+      <c r="H21" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="46"/>
+      <c r="I21" s="55"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -17171,12 +17171,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -17187,6 +17181,12 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B13:AF14">
     <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
@@ -17225,46 +17225,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
       <c r="AF1" s="12"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="48">
+      <c r="A2" s="57">
         <v>46174</v>
       </c>
       <c r="B2" s="21">
@@ -17387,14 +17387,14 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AG2" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="50"/>
-      <c r="AI2" s="50"/>
+      <c r="AG2" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="45"/>
+      <c r="AI2" s="45"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1">
-      <c r="A3" s="48"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>MO</v>
@@ -18635,14 +18635,14 @@
     <row r="15" spans="1:35" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:35">
       <c r="E16" s="42"/>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="55" t="s">
+      <c r="G16" s="59"/>
+      <c r="H16" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="62"/>
+      <c r="I16" s="47"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -18663,28 +18663,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="58" t="s">
+      <c r="Z16" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="59"/>
-      <c r="AD16" s="59"/>
-      <c r="AE16" s="59"/>
-      <c r="AF16" s="59"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="61"/>
+      <c r="AE16" s="61"/>
+      <c r="AF16" s="61"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51" t="s">
+      <c r="G17" s="58"/>
+      <c r="H17" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="63"/>
+      <c r="I17" s="49"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -18705,26 +18705,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="61"/>
-      <c r="AD17" s="61"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="61"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="63"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="63"/>
+      <c r="AE17" s="63"/>
+      <c r="AF17" s="63"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="53" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="57"/>
+      <c r="I18" s="51"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -18745,26 +18745,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="61"/>
-      <c r="AD18" s="61"/>
-      <c r="AE18" s="61"/>
-      <c r="AF18" s="61"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="63"/>
+      <c r="AC18" s="63"/>
+      <c r="AD18" s="63"/>
+      <c r="AE18" s="63"/>
+      <c r="AF18" s="63"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="54"/>
-      <c r="H19" s="53" t="s">
+      <c r="G19" s="52"/>
+      <c r="H19" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="57"/>
+      <c r="I19" s="51"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -18790,14 +18790,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="57"/>
+      <c r="I20" s="51"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -18823,14 +18823,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="44" t="s">
+      <c r="G21" s="54"/>
+      <c r="H21" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="46"/>
+      <c r="I21" s="55"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -19052,12 +19052,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -19068,6 +19062,12 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:D3 F2:J3 L2:X3 Z2:AE3">
     <cfRule type="expression" dxfId="20" priority="3">
@@ -19106,47 +19106,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="56"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="48">
+      <c r="A2" s="57">
         <v>46204</v>
       </c>
       <c r="B2" s="21">
@@ -19273,14 +19273,14 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="50"/>
-      <c r="AJ2" s="50"/>
+      <c r="AH2" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="45"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="48"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>WE</v>
@@ -20557,14 +20557,14 @@
     <row r="15" spans="1:36" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:36">
       <c r="E16" s="42"/>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="55" t="s">
+      <c r="G16" s="59"/>
+      <c r="H16" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="62"/>
+      <c r="I16" s="47"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -20585,28 +20585,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="58" t="s">
+      <c r="Z16" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="59"/>
-      <c r="AD16" s="59"/>
-      <c r="AE16" s="59"/>
-      <c r="AF16" s="59"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="61"/>
+      <c r="AE16" s="61"/>
+      <c r="AF16" s="61"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51" t="s">
+      <c r="G17" s="58"/>
+      <c r="H17" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="63"/>
+      <c r="I17" s="49"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -20627,26 +20627,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="61"/>
-      <c r="AD17" s="61"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="61"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="63"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="63"/>
+      <c r="AE17" s="63"/>
+      <c r="AF17" s="63"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="53" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="57"/>
+      <c r="I18" s="51"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -20667,26 +20667,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="61"/>
-      <c r="AD18" s="61"/>
-      <c r="AE18" s="61"/>
-      <c r="AF18" s="61"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="63"/>
+      <c r="AC18" s="63"/>
+      <c r="AD18" s="63"/>
+      <c r="AE18" s="63"/>
+      <c r="AF18" s="63"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="54"/>
-      <c r="H19" s="53" t="s">
+      <c r="G19" s="52"/>
+      <c r="H19" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="57"/>
+      <c r="I19" s="51"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -20712,14 +20712,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="57"/>
+      <c r="I20" s="51"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -20745,14 +20745,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="44" t="s">
+      <c r="G21" s="54"/>
+      <c r="H21" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="46"/>
+      <c r="I21" s="55"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -20974,12 +20974,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -20990,6 +20984,12 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:AF3">
     <cfRule type="expression" dxfId="17" priority="3">
@@ -21028,47 +21028,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="56"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="48">
+      <c r="A2" s="57">
         <v>46235</v>
       </c>
       <c r="B2" s="21">
@@ -21195,14 +21195,14 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="50"/>
-      <c r="AJ2" s="50"/>
+      <c r="AH2" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="45"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="48"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>SA</v>
@@ -22479,14 +22479,14 @@
     <row r="15" spans="1:36" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:36">
       <c r="E16" s="42"/>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="55" t="s">
+      <c r="G16" s="59"/>
+      <c r="H16" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="62"/>
+      <c r="I16" s="47"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -22507,28 +22507,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="58" t="s">
+      <c r="Z16" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="59"/>
-      <c r="AD16" s="59"/>
-      <c r="AE16" s="59"/>
-      <c r="AF16" s="59"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="61"/>
+      <c r="AE16" s="61"/>
+      <c r="AF16" s="61"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51" t="s">
+      <c r="G17" s="58"/>
+      <c r="H17" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="63"/>
+      <c r="I17" s="49"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -22549,26 +22549,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="61"/>
-      <c r="AD17" s="61"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="61"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="63"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="63"/>
+      <c r="AE17" s="63"/>
+      <c r="AF17" s="63"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="53" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="57"/>
+      <c r="I18" s="51"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -22589,26 +22589,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="61"/>
-      <c r="AD18" s="61"/>
-      <c r="AE18" s="61"/>
-      <c r="AF18" s="61"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="63"/>
+      <c r="AC18" s="63"/>
+      <c r="AD18" s="63"/>
+      <c r="AE18" s="63"/>
+      <c r="AF18" s="63"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="54"/>
-      <c r="H19" s="53" t="s">
+      <c r="G19" s="52"/>
+      <c r="H19" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="57"/>
+      <c r="I19" s="51"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -22634,14 +22634,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="57"/>
+      <c r="I20" s="51"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -22667,14 +22667,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="44" t="s">
+      <c r="G21" s="54"/>
+      <c r="H21" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="46"/>
+      <c r="I21" s="55"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -22896,12 +22896,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -22912,6 +22906,12 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:O3 Q2:AF3">
     <cfRule type="expression" dxfId="14" priority="3">
@@ -22950,46 +22950,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
       <c r="AF1" s="12"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="48">
+      <c r="A2" s="57">
         <v>46266</v>
       </c>
       <c r="B2" s="21">
@@ -23112,14 +23112,14 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AG2" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="50"/>
-      <c r="AI2" s="50"/>
+      <c r="AG2" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="45"/>
+      <c r="AI2" s="45"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1">
-      <c r="A3" s="48"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>TU</v>
@@ -24360,14 +24360,14 @@
     <row r="15" spans="1:35" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:35">
       <c r="E16" s="42"/>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="56"/>
-      <c r="H16" s="55" t="s">
+      <c r="G16" s="59"/>
+      <c r="H16" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="62"/>
+      <c r="I16" s="47"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -24388,28 +24388,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="58" t="s">
+      <c r="Z16" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="59"/>
-      <c r="AD16" s="59"/>
-      <c r="AE16" s="59"/>
-      <c r="AF16" s="59"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="61"/>
+      <c r="AE16" s="61"/>
+      <c r="AF16" s="61"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51" t="s">
+      <c r="G17" s="58"/>
+      <c r="H17" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="63"/>
+      <c r="I17" s="49"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -24430,26 +24430,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="61"/>
-      <c r="AD17" s="61"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="61"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="63"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="63"/>
+      <c r="AE17" s="63"/>
+      <c r="AF17" s="63"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="53" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="57"/>
+      <c r="I18" s="51"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -24470,26 +24470,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="61"/>
-      <c r="AD18" s="61"/>
-      <c r="AE18" s="61"/>
-      <c r="AF18" s="61"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="63"/>
+      <c r="AB18" s="63"/>
+      <c r="AC18" s="63"/>
+      <c r="AD18" s="63"/>
+      <c r="AE18" s="63"/>
+      <c r="AF18" s="63"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="54"/>
-      <c r="H19" s="53" t="s">
+      <c r="G19" s="52"/>
+      <c r="H19" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="57"/>
+      <c r="I19" s="51"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -24515,14 +24515,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="57"/>
+      <c r="I20" s="51"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -24548,14 +24548,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="44" t="s">
+      <c r="G21" s="54"/>
+      <c r="H21" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="46"/>
+      <c r="I21" s="55"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -24777,12 +24777,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -24793,6 +24787,12 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:AE3">
     <cfRule type="expression" dxfId="11" priority="3">
@@ -24813,6 +24813,68 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
+      <UserInfo>
+        <DisplayName>SANTOS, SOFIA</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CASTRO, MARIANA</DisplayName>
+        <AccountId>116</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GASPAR, DIANA</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TATO, ELISABETE</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>FONTES, ALICE</DisplayName>
+        <AccountId>88</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BASILIO, BRUNO</DisplayName>
+        <AccountId>65</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MIRANDA, ANTONIO</DisplayName>
+        <AccountId>356</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2cdea53bbbbe1c592d4ed0089fc04525">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c0fb91ccd09afdd2cf070cd91e44e663" ns2:_="" ns3:_="">
     <xsd:import namespace="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c"/>
@@ -25053,70 +25115,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
-      <UserInfo>
-        <DisplayName>SANTOS, SOFIA</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CASTRO, MARIANA</DisplayName>
-        <AccountId>116</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GASPAR, DIANA</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TATO, ELISABETE</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>FONTES, ALICE</DisplayName>
-        <AccountId>88</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BASILIO, BRUNO</DisplayName>
-        <AccountId>65</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MIRANDA, ANTONIO</DisplayName>
-        <AccountId>356</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29B84BB2-0D53-4A94-BCB9-BA0A420A2CD1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25124,7 +25124,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29B84BB2-0D53-4A94-BCB9-BA0A420A2CD1}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Update files and calendar (2026-02-03 19:11:42 UTC)
</commit_message>
<xml_diff>
--- a/files/IT_2026.xlsx
+++ b/files/IT_2026.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29721"/>
   <fileSharing readOnlyRecommended="1" userName="ALEXANDRE, LUISA" algorithmName="SHA-512" hashValue="Adf9lh9ReIucWlaaerszpKKTBJ1wqwczuUrc7Pxi/LtOOgKn18lrTzx/X3SDZIrlwuYvDSYptHSGSM48KU7dCQ==" saltValue="KG7kan4hwKZZufg2n+VohQ==" spinCount="100000"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11,7 +11,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{991245FC-07BC-4015-BDEF-4EED57848F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="11" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN" sheetId="86" r:id="rId1"/>
@@ -802,33 +802,6 @@
     <xf numFmtId="0" fontId="4" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -844,10 +817,31 @@
     <xf numFmtId="17" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -861,6 +855,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1606,40 +1606,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
@@ -1650,7 +1650,7 @@
       <c r="AN1" s="12"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="57">
+      <c r="A2" s="48">
         <v>46023</v>
       </c>
       <c r="B2" s="23">
@@ -1777,19 +1777,19 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="45"/>
-      <c r="AL2" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="45"/>
-      <c r="AN2" s="45"/>
+      <c r="AH2" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="50"/>
+      <c r="AJ2" s="50"/>
+      <c r="AL2" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="50"/>
+      <c r="AN2" s="50"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1">
-      <c r="A3" s="57"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="23" t="str">
         <f t="shared" ref="B3:AF3" si="1">UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>TH</v>
@@ -3156,14 +3156,14 @@
     <row r="15" spans="1:40" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:40">
       <c r="E16" s="42"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="46" t="s">
+      <c r="G16" s="56"/>
+      <c r="H16" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="47"/>
+      <c r="I16" s="62"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -3184,28 +3184,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="60" t="s">
+      <c r="Z16" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="61"/>
-      <c r="AF16" s="61"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="59"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="59"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="58"/>
-      <c r="H17" s="48" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="49"/>
+      <c r="I17" s="63"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -3226,26 +3226,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="62"/>
-      <c r="AA17" s="63"/>
-      <c r="AB17" s="63"/>
-      <c r="AC17" s="63"/>
-      <c r="AD17" s="63"/>
-      <c r="AE17" s="63"/>
-      <c r="AF17" s="63"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="50" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="51"/>
+      <c r="I18" s="57"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -3266,26 +3266,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="63"/>
-      <c r="AC18" s="63"/>
-      <c r="AD18" s="63"/>
-      <c r="AE18" s="63"/>
-      <c r="AF18" s="63"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="50" t="s">
+      <c r="F19" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="50" t="s">
+      <c r="G19" s="54"/>
+      <c r="H19" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="51"/>
+      <c r="I19" s="57"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -3311,14 +3311,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="50" t="s">
+      <c r="G20" s="54"/>
+      <c r="H20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="51"/>
+      <c r="I20" s="57"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -3344,14 +3344,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="45"/>
+      <c r="H21" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="46"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -3573,6 +3573,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="A1:AF1"/>
@@ -3584,12 +3590,6 @@
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="Z16:AF18"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
   </mergeCells>
   <conditionalFormatting sqref="B13:AF14">
     <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
@@ -3628,47 +3628,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="57">
+      <c r="A2" s="48">
         <v>46296</v>
       </c>
       <c r="B2" s="21">
@@ -3795,14 +3795,14 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="45"/>
+      <c r="AH2" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="50"/>
+      <c r="AJ2" s="50"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="57"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>TH</v>
@@ -4146,7 +4146,7 @@
       </c>
       <c r="AH5" s="6">
         <f>SEP!AI5</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AI5" s="15">
         <f t="shared" ref="AI5:AI11" si="3">COUNTIF(B5:AF5,"U")</f>
@@ -4154,7 +4154,7 @@
       </c>
       <c r="AJ5" s="15">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="15" customHeight="1">
@@ -5079,14 +5079,14 @@
     <row r="15" spans="1:36" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:36">
       <c r="E16" s="42"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="46" t="s">
+      <c r="G16" s="56"/>
+      <c r="H16" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="47"/>
+      <c r="I16" s="62"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -5107,28 +5107,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="60" t="s">
+      <c r="Z16" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="61"/>
-      <c r="AF16" s="61"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="59"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="59"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="58"/>
-      <c r="H17" s="48" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="49"/>
+      <c r="I17" s="63"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -5149,26 +5149,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="62"/>
-      <c r="AA17" s="63"/>
-      <c r="AB17" s="63"/>
-      <c r="AC17" s="63"/>
-      <c r="AD17" s="63"/>
-      <c r="AE17" s="63"/>
-      <c r="AF17" s="63"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="50" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="51"/>
+      <c r="I18" s="57"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -5189,26 +5189,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="63"/>
-      <c r="AC18" s="63"/>
-      <c r="AD18" s="63"/>
-      <c r="AE18" s="63"/>
-      <c r="AF18" s="63"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="50" t="s">
+      <c r="F19" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="50" t="s">
+      <c r="G19" s="54"/>
+      <c r="H19" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="51"/>
+      <c r="I19" s="57"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -5234,14 +5234,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="50" t="s">
+      <c r="G20" s="54"/>
+      <c r="H20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="51"/>
+      <c r="I20" s="57"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -5267,14 +5267,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="45"/>
+      <c r="H21" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="46"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -5496,6 +5496,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -5506,12 +5512,6 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:E3 G2:AF3">
     <cfRule type="expression" dxfId="8" priority="3">
@@ -5550,46 +5550,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
       <c r="AF1" s="12"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="57">
+      <c r="A2" s="48">
         <v>46327</v>
       </c>
       <c r="B2" s="23">
@@ -5712,14 +5712,14 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="45"/>
-      <c r="AI2" s="45"/>
+      <c r="AG2" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="50"/>
+      <c r="AI2" s="50"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1">
-      <c r="A3" s="57"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="23" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>SU</v>
@@ -6053,7 +6053,7 @@
       </c>
       <c r="AG5" s="6">
         <f>OCT!AJ5</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AH5" s="15">
         <f t="shared" ref="AH5:AH11" si="3">COUNTIF(B5:AE5,"U")</f>
@@ -6061,7 +6061,7 @@
       </c>
       <c r="AI5" s="15">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="15" customHeight="1">
@@ -6960,14 +6960,14 @@
     <row r="15" spans="1:35" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:35">
       <c r="E16" s="42"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="46" t="s">
+      <c r="G16" s="56"/>
+      <c r="H16" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="47"/>
+      <c r="I16" s="62"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -6988,28 +6988,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="60" t="s">
+      <c r="Z16" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="61"/>
-      <c r="AF16" s="61"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="59"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="59"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="58"/>
-      <c r="H17" s="48" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="49"/>
+      <c r="I17" s="63"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -7030,26 +7030,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="62"/>
-      <c r="AA17" s="63"/>
-      <c r="AB17" s="63"/>
-      <c r="AC17" s="63"/>
-      <c r="AD17" s="63"/>
-      <c r="AE17" s="63"/>
-      <c r="AF17" s="63"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="50" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="51"/>
+      <c r="I18" s="57"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -7070,26 +7070,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="63"/>
-      <c r="AC18" s="63"/>
-      <c r="AD18" s="63"/>
-      <c r="AE18" s="63"/>
-      <c r="AF18" s="63"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="50" t="s">
+      <c r="F19" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="50" t="s">
+      <c r="G19" s="54"/>
+      <c r="H19" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="51"/>
+      <c r="I19" s="57"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -7115,14 +7115,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="50" t="s">
+      <c r="G20" s="54"/>
+      <c r="H20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="51"/>
+      <c r="I20" s="57"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -7148,14 +7148,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="45"/>
+      <c r="H21" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="46"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -7377,6 +7377,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -7387,12 +7393,6 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B13:AE14">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
@@ -7431,47 +7431,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="57">
+      <c r="A2" s="48">
         <v>46357</v>
       </c>
       <c r="B2" s="23">
@@ -7598,14 +7598,14 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="45"/>
+      <c r="AH2" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="50"/>
+      <c r="AJ2" s="50"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="57"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="23" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>TU</v>
@@ -7949,7 +7949,7 @@
       </c>
       <c r="AH5" s="6">
         <f>NOV!AI5</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AI5" s="15">
         <f t="shared" ref="AI5:AI11" si="3">COUNTIF(B5:AF5,"U")</f>
@@ -7957,7 +7957,7 @@
       </c>
       <c r="AJ5" s="15">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="15" customHeight="1">
@@ -8882,14 +8882,14 @@
     <row r="15" spans="1:36" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:36">
       <c r="E16" s="42"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="46" t="s">
+      <c r="G16" s="56"/>
+      <c r="H16" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="47"/>
+      <c r="I16" s="62"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -8910,28 +8910,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="60" t="s">
+      <c r="Z16" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="61"/>
-      <c r="AF16" s="61"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="59"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="59"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="58"/>
-      <c r="H17" s="48" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="49"/>
+      <c r="I17" s="63"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -8952,26 +8952,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="62"/>
-      <c r="AA17" s="63"/>
-      <c r="AB17" s="63"/>
-      <c r="AC17" s="63"/>
-      <c r="AD17" s="63"/>
-      <c r="AE17" s="63"/>
-      <c r="AF17" s="63"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="50" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="51"/>
+      <c r="I18" s="57"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -8992,26 +8992,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="63"/>
-      <c r="AC18" s="63"/>
-      <c r="AD18" s="63"/>
-      <c r="AE18" s="63"/>
-      <c r="AF18" s="63"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="50" t="s">
+      <c r="F19" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="50" t="s">
+      <c r="G19" s="54"/>
+      <c r="H19" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="51"/>
+      <c r="I19" s="57"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -9037,14 +9037,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="50" t="s">
+      <c r="G20" s="54"/>
+      <c r="H20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="51"/>
+      <c r="I20" s="57"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -9070,14 +9070,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="45"/>
+      <c r="H21" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="46"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -9299,6 +9299,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -9309,12 +9315,6 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B13:AF14">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -9340,7 +9340,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5:G5"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -9353,37 +9353,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
       <c r="AD1" s="12"/>
       <c r="AE1" s="12"/>
       <c r="AF1" s="12"/>
@@ -9394,7 +9394,7 @@
       <c r="AK1" s="12"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="57">
+      <c r="A2" s="48">
         <v>46054</v>
       </c>
       <c r="B2" s="21">
@@ -9509,19 +9509,19 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AE2" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="45"/>
-      <c r="AG2" s="45"/>
-      <c r="AI2" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="45"/>
-      <c r="AK2" s="45"/>
+      <c r="AE2" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="50"/>
+      <c r="AG2" s="50"/>
+      <c r="AI2" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="50"/>
+      <c r="AK2" s="50"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1">
-      <c r="A3" s="57"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>SU</v>
@@ -9782,11 +9782,11 @@
       <c r="E5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>9</v>
+      <c r="F5" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>18</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>8</v>
@@ -9872,11 +9872,11 @@
       </c>
       <c r="AJ5" s="15">
         <f t="shared" ref="AJ4:AJ11" si="5">COUNTIF(B5:AC5,"U")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK5" s="15">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:37" ht="15" customHeight="1">
@@ -10796,14 +10796,14 @@
     <row r="15" spans="1:37" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:37">
       <c r="E16" s="42"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="46" t="s">
+      <c r="G16" s="56"/>
+      <c r="H16" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="47"/>
+      <c r="I16" s="62"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -10824,28 +10824,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="60" t="s">
+      <c r="Z16" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="61"/>
-      <c r="AF16" s="61"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="59"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="59"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="58"/>
-      <c r="H17" s="48" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="49"/>
+      <c r="I17" s="63"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -10866,26 +10866,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="62"/>
-      <c r="AA17" s="63"/>
-      <c r="AB17" s="63"/>
-      <c r="AC17" s="63"/>
-      <c r="AD17" s="63"/>
-      <c r="AE17" s="63"/>
-      <c r="AF17" s="63"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="50" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="51"/>
+      <c r="I18" s="57"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -10906,26 +10906,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="63"/>
-      <c r="AC18" s="63"/>
-      <c r="AD18" s="63"/>
-      <c r="AE18" s="63"/>
-      <c r="AF18" s="63"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="50" t="s">
+      <c r="F19" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="50" t="s">
+      <c r="G19" s="54"/>
+      <c r="H19" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="51"/>
+      <c r="I19" s="57"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -10951,14 +10951,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="50" t="s">
+      <c r="G20" s="54"/>
+      <c r="H20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="51"/>
+      <c r="I20" s="57"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -10984,14 +10984,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="45"/>
+      <c r="H21" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="46"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -11213,6 +11213,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:AC1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -11223,13 +11230,6 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A1:AC1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:Q3 S2:AC3">
     <cfRule type="expression" dxfId="32" priority="5">
@@ -11268,40 +11268,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
@@ -11312,7 +11312,7 @@
       <c r="AN1" s="12"/>
     </row>
     <row r="2" spans="1:40" ht="15" customHeight="1">
-      <c r="A2" s="57">
+      <c r="A2" s="48">
         <v>46082</v>
       </c>
       <c r="B2" s="21">
@@ -11439,19 +11439,19 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="45"/>
-      <c r="AL2" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM2" s="45"/>
-      <c r="AN2" s="45"/>
+      <c r="AH2" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="50"/>
+      <c r="AJ2" s="50"/>
+      <c r="AL2" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="50"/>
+      <c r="AN2" s="50"/>
     </row>
     <row r="3" spans="1:40" ht="15" customHeight="1">
-      <c r="A3" s="57"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>SU</v>
@@ -11828,7 +11828,7 @@
       </c>
       <c r="AL5" s="6">
         <f>FEB!AK5</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AM5" s="15">
         <f t="shared" ref="AM5:AM11" si="5">COUNTIF(B5:AF5,"U")</f>
@@ -11836,7 +11836,7 @@
       </c>
       <c r="AN5" s="15">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:40" ht="15" customHeight="1">
@@ -12834,14 +12834,14 @@
     <row r="15" spans="1:40" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:40">
       <c r="E16" s="42"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="46" t="s">
+      <c r="G16" s="56"/>
+      <c r="H16" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="47"/>
+      <c r="I16" s="62"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -12862,28 +12862,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="60" t="s">
+      <c r="Z16" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="61"/>
-      <c r="AF16" s="61"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="59"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="59"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="58"/>
-      <c r="H17" s="48" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="49"/>
+      <c r="I17" s="63"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -12904,26 +12904,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="62"/>
-      <c r="AA17" s="63"/>
-      <c r="AB17" s="63"/>
-      <c r="AC17" s="63"/>
-      <c r="AD17" s="63"/>
-      <c r="AE17" s="63"/>
-      <c r="AF17" s="63"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="50" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="51"/>
+      <c r="I18" s="57"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -12944,26 +12944,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="63"/>
-      <c r="AC18" s="63"/>
-      <c r="AD18" s="63"/>
-      <c r="AE18" s="63"/>
-      <c r="AF18" s="63"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="50" t="s">
+      <c r="F19" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="50" t="s">
+      <c r="G19" s="54"/>
+      <c r="H19" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="51"/>
+      <c r="I19" s="57"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -12989,14 +12989,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="50" t="s">
+      <c r="G20" s="54"/>
+      <c r="H20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="51"/>
+      <c r="I20" s="57"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -13022,14 +13022,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="45"/>
+      <c r="H21" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="46"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -13251,6 +13251,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -13261,13 +13268,6 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:AF3">
     <cfRule type="expression" dxfId="29" priority="5">
@@ -13306,39 +13306,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="15" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
       <c r="AF1" s="12"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
@@ -13349,7 +13349,7 @@
       <c r="AM1" s="12"/>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1">
-      <c r="A2" s="57">
+      <c r="A2" s="48">
         <v>46113</v>
       </c>
       <c r="B2" s="21">
@@ -13472,19 +13472,19 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="45"/>
-      <c r="AI2" s="45"/>
-      <c r="AK2" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="45"/>
-      <c r="AM2" s="45"/>
+      <c r="AG2" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="50"/>
+      <c r="AI2" s="50"/>
+      <c r="AK2" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="50"/>
+      <c r="AM2" s="50"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1">
-      <c r="A3" s="57"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>WE</v>
@@ -13851,7 +13851,7 @@
       </c>
       <c r="AK5" s="6">
         <f>MAR!AN5</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AL5" s="15">
         <f t="shared" ref="AL5:AL11" si="5">COUNTIF(B5:AE5,"U")</f>
@@ -13859,7 +13859,7 @@
       </c>
       <c r="AM5" s="15">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:39" ht="15" customHeight="1">
@@ -14831,14 +14831,14 @@
     <row r="15" spans="1:39" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:39">
       <c r="E16" s="42"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="46" t="s">
+      <c r="G16" s="56"/>
+      <c r="H16" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="47"/>
+      <c r="I16" s="62"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -14859,28 +14859,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="60" t="s">
+      <c r="Z16" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="61"/>
-      <c r="AF16" s="61"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="59"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="59"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="58"/>
-      <c r="H17" s="48" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="49"/>
+      <c r="I17" s="63"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -14901,26 +14901,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="62"/>
-      <c r="AA17" s="63"/>
-      <c r="AB17" s="63"/>
-      <c r="AC17" s="63"/>
-      <c r="AD17" s="63"/>
-      <c r="AE17" s="63"/>
-      <c r="AF17" s="63"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="50" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="51"/>
+      <c r="I18" s="57"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -14941,26 +14941,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="63"/>
-      <c r="AC18" s="63"/>
-      <c r="AD18" s="63"/>
-      <c r="AE18" s="63"/>
-      <c r="AF18" s="63"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="50" t="s">
+      <c r="F19" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="50" t="s">
+      <c r="G19" s="54"/>
+      <c r="H19" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="51"/>
+      <c r="I19" s="57"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -14986,14 +14986,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="50" t="s">
+      <c r="G20" s="54"/>
+      <c r="H20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="51"/>
+      <c r="I20" s="57"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -15019,14 +15019,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="45"/>
+      <c r="H21" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="46"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -15248,6 +15248,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="AK2:AM2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -15258,13 +15265,6 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:C3 E2:E3 G2:Y3 AA2:AE3">
     <cfRule type="expression" dxfId="26" priority="3">
@@ -15303,47 +15303,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="57">
+      <c r="A2" s="48">
         <v>46143</v>
       </c>
       <c r="B2" s="23">
@@ -15470,14 +15470,14 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="45"/>
+      <c r="AH2" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="50"/>
+      <c r="AJ2" s="50"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="57"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="23" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>FR</v>
@@ -15821,7 +15821,7 @@
       </c>
       <c r="AH5" s="6">
         <f>APR!AM5</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AI5" s="15">
         <f t="shared" ref="AI5:AI11" si="9">COUNTIF(B5:AF5,"U")</f>
@@ -15829,7 +15829,7 @@
       </c>
       <c r="AJ5" s="15">
         <f t="shared" si="8"/>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="15" customHeight="1">
@@ -16754,14 +16754,14 @@
     <row r="15" spans="1:36" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:36">
       <c r="E16" s="42"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="46" t="s">
+      <c r="G16" s="56"/>
+      <c r="H16" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="47"/>
+      <c r="I16" s="62"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -16782,28 +16782,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="60" t="s">
+      <c r="Z16" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="61"/>
-      <c r="AF16" s="61"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="59"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="59"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="58"/>
-      <c r="H17" s="48" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="49"/>
+      <c r="I17" s="63"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -16824,26 +16824,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="62"/>
-      <c r="AA17" s="63"/>
-      <c r="AB17" s="63"/>
-      <c r="AC17" s="63"/>
-      <c r="AD17" s="63"/>
-      <c r="AE17" s="63"/>
-      <c r="AF17" s="63"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="50" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="51"/>
+      <c r="I18" s="57"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -16864,26 +16864,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="63"/>
-      <c r="AC18" s="63"/>
-      <c r="AD18" s="63"/>
-      <c r="AE18" s="63"/>
-      <c r="AF18" s="63"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="50" t="s">
+      <c r="F19" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="50" t="s">
+      <c r="G19" s="54"/>
+      <c r="H19" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="51"/>
+      <c r="I19" s="57"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -16909,14 +16909,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="50" t="s">
+      <c r="G20" s="54"/>
+      <c r="H20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="51"/>
+      <c r="I20" s="57"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -16942,14 +16942,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="45"/>
+      <c r="H21" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="46"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -17171,6 +17171,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -17181,12 +17187,6 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B13:AF14">
     <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
@@ -17225,46 +17225,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
       <c r="AF1" s="12"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="57">
+      <c r="A2" s="48">
         <v>46174</v>
       </c>
       <c r="B2" s="21">
@@ -17387,14 +17387,14 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="45"/>
-      <c r="AI2" s="45"/>
+      <c r="AG2" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="50"/>
+      <c r="AI2" s="50"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1">
-      <c r="A3" s="57"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>MO</v>
@@ -17728,7 +17728,7 @@
       </c>
       <c r="AG5" s="6">
         <f>MAY!AJ5</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AH5" s="15">
         <f t="shared" ref="AH5:AH11" si="3">COUNTIF(B5:AE5,"U")</f>
@@ -17736,7 +17736,7 @@
       </c>
       <c r="AI5" s="15">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="15" customHeight="1">
@@ -18635,14 +18635,14 @@
     <row r="15" spans="1:35" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:35">
       <c r="E16" s="42"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="46" t="s">
+      <c r="G16" s="56"/>
+      <c r="H16" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="47"/>
+      <c r="I16" s="62"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -18663,28 +18663,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="60" t="s">
+      <c r="Z16" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="61"/>
-      <c r="AF16" s="61"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="59"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="59"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="58"/>
-      <c r="H17" s="48" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="49"/>
+      <c r="I17" s="63"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -18705,26 +18705,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="62"/>
-      <c r="AA17" s="63"/>
-      <c r="AB17" s="63"/>
-      <c r="AC17" s="63"/>
-      <c r="AD17" s="63"/>
-      <c r="AE17" s="63"/>
-      <c r="AF17" s="63"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="50" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="51"/>
+      <c r="I18" s="57"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -18745,26 +18745,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="63"/>
-      <c r="AC18" s="63"/>
-      <c r="AD18" s="63"/>
-      <c r="AE18" s="63"/>
-      <c r="AF18" s="63"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="50" t="s">
+      <c r="F19" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="50" t="s">
+      <c r="G19" s="54"/>
+      <c r="H19" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="51"/>
+      <c r="I19" s="57"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -18790,14 +18790,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="50" t="s">
+      <c r="G20" s="54"/>
+      <c r="H20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="51"/>
+      <c r="I20" s="57"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -18823,14 +18823,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="45"/>
+      <c r="H21" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="46"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -19052,6 +19052,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -19062,12 +19068,6 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:D3 F2:J3 L2:X3 Z2:AE3">
     <cfRule type="expression" dxfId="20" priority="3">
@@ -19106,47 +19106,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="57">
+      <c r="A2" s="48">
         <v>46204</v>
       </c>
       <c r="B2" s="21">
@@ -19273,14 +19273,14 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="45"/>
+      <c r="AH2" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="50"/>
+      <c r="AJ2" s="50"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="57"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>WE</v>
@@ -19624,7 +19624,7 @@
       </c>
       <c r="AH5" s="6">
         <f>JUN!AI5</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AI5" s="15">
         <f t="shared" ref="AI5:AI11" si="3">COUNTIF(B5:AF5,"U")</f>
@@ -19632,7 +19632,7 @@
       </c>
       <c r="AJ5" s="15">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="15" customHeight="1">
@@ -20557,14 +20557,14 @@
     <row r="15" spans="1:36" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:36">
       <c r="E16" s="42"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="46" t="s">
+      <c r="G16" s="56"/>
+      <c r="H16" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="47"/>
+      <c r="I16" s="62"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -20585,28 +20585,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="60" t="s">
+      <c r="Z16" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="61"/>
-      <c r="AF16" s="61"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="59"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="59"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="58"/>
-      <c r="H17" s="48" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="49"/>
+      <c r="I17" s="63"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -20627,26 +20627,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="62"/>
-      <c r="AA17" s="63"/>
-      <c r="AB17" s="63"/>
-      <c r="AC17" s="63"/>
-      <c r="AD17" s="63"/>
-      <c r="AE17" s="63"/>
-      <c r="AF17" s="63"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="50" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="51"/>
+      <c r="I18" s="57"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -20667,26 +20667,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="63"/>
-      <c r="AC18" s="63"/>
-      <c r="AD18" s="63"/>
-      <c r="AE18" s="63"/>
-      <c r="AF18" s="63"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="50" t="s">
+      <c r="F19" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="50" t="s">
+      <c r="G19" s="54"/>
+      <c r="H19" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="51"/>
+      <c r="I19" s="57"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -20712,14 +20712,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="50" t="s">
+      <c r="G20" s="54"/>
+      <c r="H20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="51"/>
+      <c r="I20" s="57"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -20745,14 +20745,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="45"/>
+      <c r="H21" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="46"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -20974,6 +20974,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -20984,12 +20990,6 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:AF3">
     <cfRule type="expression" dxfId="17" priority="3">
@@ -21028,47 +21028,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
       <c r="AJ1" s="12"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="57">
+      <c r="A2" s="48">
         <v>46235</v>
       </c>
       <c r="B2" s="21">
@@ -21195,14 +21195,14 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH2" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="45"/>
+      <c r="AH2" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="50"/>
+      <c r="AJ2" s="50"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="57"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>SA</v>
@@ -21546,7 +21546,7 @@
       </c>
       <c r="AH5" s="6">
         <f>JUL!AJ5</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AI5" s="15">
         <f t="shared" ref="AI5:AI11" si="3">COUNTIF(B5:AF5,"U")</f>
@@ -21554,7 +21554,7 @@
       </c>
       <c r="AJ5" s="15">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="15" customHeight="1">
@@ -22479,14 +22479,14 @@
     <row r="15" spans="1:36" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:36">
       <c r="E16" s="42"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="46" t="s">
+      <c r="G16" s="56"/>
+      <c r="H16" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="47"/>
+      <c r="I16" s="62"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -22507,28 +22507,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="60" t="s">
+      <c r="Z16" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="61"/>
-      <c r="AF16" s="61"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="59"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="59"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="58"/>
-      <c r="H17" s="48" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="49"/>
+      <c r="I17" s="63"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -22549,26 +22549,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="62"/>
-      <c r="AA17" s="63"/>
-      <c r="AB17" s="63"/>
-      <c r="AC17" s="63"/>
-      <c r="AD17" s="63"/>
-      <c r="AE17" s="63"/>
-      <c r="AF17" s="63"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="50" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="51"/>
+      <c r="I18" s="57"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -22589,26 +22589,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="63"/>
-      <c r="AC18" s="63"/>
-      <c r="AD18" s="63"/>
-      <c r="AE18" s="63"/>
-      <c r="AF18" s="63"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="50" t="s">
+      <c r="F19" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="50" t="s">
+      <c r="G19" s="54"/>
+      <c r="H19" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="51"/>
+      <c r="I19" s="57"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -22634,14 +22634,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="50" t="s">
+      <c r="G20" s="54"/>
+      <c r="H20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="51"/>
+      <c r="I20" s="57"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -22667,14 +22667,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="45"/>
+      <c r="H21" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="46"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -22896,6 +22896,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -22906,12 +22912,6 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A1:AF1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:O3 Q2:AF3">
     <cfRule type="expression" dxfId="14" priority="3">
@@ -22950,46 +22950,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
       <c r="AF1" s="12"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1">
-      <c r="A2" s="57">
+      <c r="A2" s="48">
         <v>46266</v>
       </c>
       <c r="B2" s="21">
@@ -23112,14 +23112,14 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AG2" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="45"/>
-      <c r="AI2" s="45"/>
+      <c r="AG2" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="50"/>
+      <c r="AI2" s="50"/>
     </row>
     <row r="3" spans="1:35" ht="15" customHeight="1">
-      <c r="A3" s="57"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="21" t="str">
         <f>UPPER(LEFT(TEXT(DATE(YEAR($A$2),MONTH($A$2),B2),"DDD"),2))</f>
         <v>TU</v>
@@ -23453,7 +23453,7 @@
       </c>
       <c r="AG5" s="6">
         <f>AUG!AJ5</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AH5" s="15">
         <f t="shared" ref="AH5:AH11" si="3">COUNTIF(B5:AE5,"U")</f>
@@ -23461,7 +23461,7 @@
       </c>
       <c r="AI5" s="15">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="15" customHeight="1">
@@ -24360,14 +24360,14 @@
     <row r="15" spans="1:35" ht="13.5" thickBot="1"/>
     <row r="16" spans="1:35">
       <c r="E16" s="42"/>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="46" t="s">
+      <c r="G16" s="56"/>
+      <c r="H16" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="47"/>
+      <c r="I16" s="62"/>
       <c r="M16" s="6" t="s">
         <v>8</v>
       </c>
@@ -24388,28 +24388,28 @@
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
       <c r="X16" s="28"/>
-      <c r="Z16" s="60" t="s">
+      <c r="Z16" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="61"/>
-      <c r="AF16" s="61"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="59"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="59"/>
     </row>
     <row r="17" spans="5:32">
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="58"/>
-      <c r="H17" s="48" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="49"/>
+      <c r="I17" s="63"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -24430,26 +24430,26 @@
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
       <c r="X17" s="19"/>
-      <c r="Z17" s="62"/>
-      <c r="AA17" s="63"/>
-      <c r="AB17" s="63"/>
-      <c r="AC17" s="63"/>
-      <c r="AD17" s="63"/>
-      <c r="AE17" s="63"/>
-      <c r="AF17" s="63"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
     </row>
     <row r="18" spans="5:32">
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="50" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="51"/>
+      <c r="I18" s="57"/>
       <c r="M18" s="23" t="s">
         <v>6</v>
       </c>
@@ -24470,26 +24470,26 @@
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
       <c r="X18" s="19"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="63"/>
-      <c r="AB18" s="63"/>
-      <c r="AC18" s="63"/>
-      <c r="AD18" s="63"/>
-      <c r="AE18" s="63"/>
-      <c r="AF18" s="63"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
     </row>
     <row r="19" spans="5:32">
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="50" t="s">
+      <c r="F19" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="50" t="s">
+      <c r="G19" s="54"/>
+      <c r="H19" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="51"/>
+      <c r="I19" s="57"/>
       <c r="M19" s="31" t="s">
         <v>18</v>
       </c>
@@ -24515,14 +24515,14 @@
       <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="50" t="s">
+      <c r="G20" s="54"/>
+      <c r="H20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="51"/>
+      <c r="I20" s="57"/>
       <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
@@ -24548,14 +24548,14 @@
       <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53" t="s">
+      <c r="G21" s="45"/>
+      <c r="H21" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="46"/>
       <c r="M21" s="32" t="s">
         <v>6</v>
       </c>
@@ -24777,6 +24777,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:AE1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Z16:AF18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="F21:G21"/>
@@ -24787,12 +24793,6 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="Z16:AF18"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:AE3">
     <cfRule type="expression" dxfId="11" priority="3">
@@ -24813,68 +24813,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
-      <UserInfo>
-        <DisplayName>SANTOS, SOFIA</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CASTRO, MARIANA</DisplayName>
-        <AccountId>116</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GASPAR, DIANA</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TATO, ELISABETE</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>FONTES, ALICE</DisplayName>
-        <AccountId>88</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BASILIO, BRUNO</DisplayName>
-        <AccountId>65</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MIRANDA, ANTONIO</DisplayName>
-        <AccountId>356</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EE2D3878C914646AFDAF8DB79C9CBFF" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2cdea53bbbbe1c592d4ed0089fc04525">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c" xmlns:ns3="fa453329-a4c9-4120-b786-6a0f9fa17d90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c0fb91ccd09afdd2cf070cd91e44e663" ns2:_="" ns3:_="">
     <xsd:import namespace="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c"/>
@@ -25115,8 +25053,70 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90">
+      <UserInfo>
+        <DisplayName>SANTOS, SOFIA</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CASTRO, MARIANA</DisplayName>
+        <AccountId>116</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GASPAR, DIANA</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TATO, ELISABETE</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>FONTES, ALICE</DisplayName>
+        <AccountId>88</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SILVA SANTOS, NUNO MIGUEL</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BASILIO, BRUNO</DisplayName>
+        <AccountId>65</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MIRANDA, ANTONIO</DisplayName>
+        <AccountId>356</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="fa453329-a4c9-4120-b786-6a0f9fa17d90" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3af6a4-7f71-4dc2-99e7-9db1cbaccb2c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29B84BB2-0D53-4A94-BCB9-BA0A420A2CD1}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25124,7 +25124,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29B84BB2-0D53-4A94-BCB9-BA0A420A2CD1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED20691-38BD-4744-A2B0-0BB0E052B916}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>